<commit_message>
add list of top XCI genes
</commit_message>
<xml_diff>
--- a/data/xist_top_genes.xlsx
+++ b/data/xist_top_genes.xlsx
@@ -27,7 +27,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>gene_name</t>
+  </si>
   <si>
     <t>XIST</t>
   </si>
@@ -1224,10 +1227,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1307,6 +1310,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>